<commit_message>
Ja31/29654 edited to non capital letters
</commit_message>
<xml_diff>
--- a/source_data/DNA_plates.xlsx
+++ b/source_data/DNA_plates.xlsx
@@ -1373,8 +1373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G929"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A912" workbookViewId="0">
-      <selection activeCell="I942" sqref="I942"/>
+    <sheetView tabSelected="1" topLeftCell="A600" workbookViewId="0">
+      <selection activeCell="C629" sqref="C629"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -14554,7 +14554,7 @@
         <v>62</v>
       </c>
       <c r="C628" s="1" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="D628" s="1" t="s">
         <v>8</v>
@@ -14564,7 +14564,7 @@
       </c>
       <c r="G628" s="1" t="str">
         <f t="shared" si="9"/>
-        <v>JA31/29654</v>
+        <v>Ja31/29654</v>
       </c>
     </row>
     <row r="629" spans="1:7">

</xml_diff>

<commit_message>
deleted spaces in DNA_plates file and some rows in NCBI file
</commit_message>
<xml_diff>
--- a/source_data/DNA_plates.xlsx
+++ b/source_data/DNA_plates.xlsx
@@ -1373,8 +1373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G929"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A600" workbookViewId="0">
-      <selection activeCell="C629" sqref="C629"/>
+    <sheetView tabSelected="1" topLeftCell="A508" workbookViewId="0">
+      <selection activeCell="C528" sqref="C528"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -11215,7 +11215,7 @@
         <v>97</v>
       </c>
       <c r="C469" s="1" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="D469" s="1" t="s">
         <v>8</v>
@@ -11225,7 +11225,7 @@
       </c>
       <c r="G469" s="1" t="str">
         <f t="shared" si="7"/>
-        <v>Fe1 /14192</v>
+        <v>Fe1/14192</v>
       </c>
     </row>
     <row r="470" spans="1:7">
@@ -12433,7 +12433,7 @@
         <v>57</v>
       </c>
       <c r="C527" s="1" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="D527" s="1" t="s">
         <v>8</v>
@@ -12443,7 +12443,7 @@
       </c>
       <c r="G527" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>Fe1 /14287</v>
+        <v>Fe1/14287</v>
       </c>
     </row>
     <row r="528" spans="1:7">
@@ -15751,7 +15751,7 @@
         <v>21</v>
       </c>
       <c r="C685" s="1" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="D685" s="1" t="s">
         <v>8</v>
@@ -15761,7 +15761,7 @@
       </c>
       <c r="G685" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>Fe1 /14160</v>
+        <v>Fe1/14160</v>
       </c>
     </row>
     <row r="686" spans="1:7">
@@ -17347,7 +17347,7 @@
         <v>101</v>
       </c>
       <c r="C761" s="1" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="D761" s="1" t="s">
         <v>8</v>
@@ -17357,7 +17357,7 @@
       </c>
       <c r="G761" s="1" t="str">
         <f t="shared" si="11"/>
-        <v>Fe1 /14273</v>
+        <v>Fe1/14273</v>
       </c>
     </row>
     <row r="762" spans="1:7">

</xml_diff>

<commit_message>
corrected some collection dates and deleted some extra rows
</commit_message>
<xml_diff>
--- a/source_data/DNA_plates.xlsx
+++ b/source_data/DNA_plates.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17360" windowHeight="14020" tabRatio="991"/>
+    <workbookView xWindow="9820" yWindow="0" windowWidth="17360" windowHeight="14020" tabRatio="991"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1448,8 +1448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G929"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A730" workbookViewId="0">
-      <selection activeCell="E764" sqref="E764"/>
+    <sheetView tabSelected="1" topLeftCell="A572" workbookViewId="0">
+      <selection activeCell="E609" sqref="E609"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
edited the chem_dates where wrong
</commit_message>
<xml_diff>
--- a/source_data/DNA_plates.xlsx
+++ b/source_data/DNA_plates.xlsx
@@ -1075,8 +1075,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1100,7 +1102,7 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1109,6 +1111,7 @@
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1117,6 +1120,7 @@
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1448,8 +1452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G929"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A572" workbookViewId="0">
-      <selection activeCell="E609" sqref="E609"/>
+    <sheetView tabSelected="1" topLeftCell="A426" workbookViewId="0">
+      <selection activeCell="D433" sqref="D433"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>

</xml_diff>